<commit_message>
Add functions for SP and OD paths, update CPI-U-RS data (#24)
Co-authored-by: LuisNnz <97481336+LuisNnz@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data-raw/cpi_u_rs.xlsx
+++ b/data-raw/cpi_u_rs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\RS2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\RS2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA8F765-4C68-405C-A83F-3D99460B9C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7944"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -266,6 +267,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -301,6 +319,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -476,11 +511,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O1"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2540,6 +2575,50 @@
         <v>381.2</v>
       </c>
     </row>
+    <row r="51" spans="1:14" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>2021</v>
+      </c>
+      <c r="B51" s="7">
+        <v>385.2</v>
+      </c>
+      <c r="C51" s="7">
+        <v>387.3</v>
+      </c>
+      <c r="D51" s="8">
+        <v>390</v>
+      </c>
+      <c r="E51" s="8">
+        <v>393.2</v>
+      </c>
+      <c r="F51" s="7">
+        <v>396.4</v>
+      </c>
+      <c r="G51" s="7">
+        <v>400</v>
+      </c>
+      <c r="H51" s="7">
+        <v>402</v>
+      </c>
+      <c r="I51" s="7">
+        <v>402.8</v>
+      </c>
+      <c r="J51" s="7">
+        <v>403.9</v>
+      </c>
+      <c r="K51" s="7">
+        <v>407.2</v>
+      </c>
+      <c r="L51" s="7">
+        <v>409.2</v>
+      </c>
+      <c r="M51" s="7">
+        <v>410.5</v>
+      </c>
+      <c r="N51" s="7">
+        <v>399</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:XFD3"/>

</xml_diff>